<commit_message>
user hidden and production edited by admins
</commit_message>
<xml_diff>
--- a/ProjectX/wwwroot/Samplefile/benefits.xlsx
+++ b/ProjectX/wwwroot/Samplefile/benefits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamad Tormos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBB54F8-DA0A-42B0-8167-3C61E8FC73E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1F7A24-7894-4E78-B046-9C03C73D8B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="benefits" sheetId="1" r:id="rId1"/>
@@ -20,30 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>B_Limit</t>
-  </si>
-  <si>
-    <t>B_Is_Plus</t>
-  </si>
-  <si>
-    <t>B_Additional_Benefits</t>
-  </si>
-  <si>
-    <t>B_Additional_Benefits_Format</t>
   </si>
   <si>
     <t>B_Id</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>B_Title</t>
   </si>
   <si>
-    <t>#</t>
+    <t>mousa</t>
   </si>
   <si>
-    <t>no</t>
+    <t>sami</t>
   </si>
 </sst>
 </file>
@@ -884,63 +875,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>1234</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>1000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>